<commit_message>
basics on functions in R
</commit_message>
<xml_diff>
--- a/rawData/loan.xlsx
+++ b/rawData/loan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ktrei\Documents\senior2022\IT513DataMining&amp;Visualization\DataVProj\DataVisualization\rawData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4F986EA-75D7-4365-85D6-3CFD1B799E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B878B8E0-8EC4-47DA-A2C7-CFA1CFCEE84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{43B95241-8E43-4899-84AE-1B4D76D1200B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="13">
   <si>
     <t>age</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>excellent</t>
-  </si>
-  <si>
-    <t>ecvellent</t>
   </si>
 </sst>
 </file>
@@ -429,7 +426,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -645,7 +642,7 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>

</xml_diff>